<commit_message>
I updated all the graphs and added a word counter
</commit_message>
<xml_diff>
--- a/Hjemsendelse 16-11-2025.xlsx
+++ b/Hjemsendelse 16-11-2025.xlsx
@@ -1,35 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hansandersen/Desktop/UNI/Bachelor/Bachelor/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6E248A-A0F0-E344-9F67-9A804F4230BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Ordnet" sheetId="1" r:id="rId1"/>
-    <sheet name="Forskellige_se" sheetId="2" r:id="rId2"/>
+    <sheet r:id="rId1" sheetId="1" name="Ordnet"/>
+    <sheet r:id="rId2" sheetId="2" name="Forskellige_se"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -219,14 +200,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -262,29 +250,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -295,10 +292,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -336,71 +333,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -428,7 +425,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -451,11 +448,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -464,13 +461,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -480,7 +477,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -489,7 +486,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -498,7 +495,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -506,10 +503,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -574,351 +571,272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="9.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="str">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+      <c r="A1" s="4">
         <f>Forskellige_se!A1</f>
-        <v>bw</v>
-      </c>
-      <c r="B1" s="2" t="str">
+      </c>
+      <c r="B1" s="5">
         <f>Forskellige_se!E1</f>
-        <v>cl_sogn_lin</v>
-      </c>
-      <c r="C1" s="2" t="str">
+      </c>
+      <c r="C1" s="5">
         <f>Forskellige_se!F1</f>
-        <v>cl_sogn_quad</v>
-      </c>
-      <c r="D1" s="2" t="str">
+      </c>
+      <c r="D1" s="5">
         <f>Forskellige_se!C1</f>
-        <v>cl_komkod_lin</v>
-      </c>
-      <c r="E1" s="2" t="str">
+      </c>
+      <c r="E1" s="5">
         <f>Forskellige_se!D1</f>
-        <v>cl_komkod_quad</v>
-      </c>
-      <c r="F1" s="2" t="str">
+      </c>
+      <c r="F1" s="5">
         <f>Forskellige_se!G1</f>
-        <v>cl_kvm_lin</v>
-      </c>
-      <c r="G1" s="2" t="str">
+      </c>
+      <c r="G1" s="5">
         <f>Forskellige_se!H1</f>
-        <v>cl_kvm_quad</v>
-      </c>
-      <c r="H1" s="2" t="str">
+      </c>
+      <c r="H1" s="5">
         <f>Forskellige_se!I1</f>
-        <v>robust_lin</v>
-      </c>
-      <c r="I1" s="2" t="str">
+      </c>
+      <c r="I1" s="5">
         <f>Forskellige_se!J1</f>
-        <v>robust_quad</v>
-      </c>
-      <c r="J1" s="2" t="str">
+      </c>
+      <c r="J1" s="5">
         <f>Forskellige_se!K1</f>
-        <v>conv_lin</v>
-      </c>
-      <c r="K1" s="2" t="str">
+      </c>
+      <c r="K1" s="5">
         <f>Forskellige_se!L1</f>
-        <v>conv_quad</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+      <c r="A2" s="4">
         <f>Forskellige_se!A2</f>
-        <v>0.5*h_mse</v>
-      </c>
-      <c r="B2" s="3" t="str">
+      </c>
+      <c r="B2" s="6">
         <f>Forskellige_se!E2</f>
-        <v>2.887***</v>
-      </c>
-      <c r="C2" s="3" t="str">
+      </c>
+      <c r="C2" s="6">
         <f>Forskellige_se!F4</f>
-        <v>4.635</v>
-      </c>
-      <c r="D2" s="3" t="str">
+      </c>
+      <c r="D2" s="6">
         <f>Forskellige_se!C2</f>
-        <v>2.887**</v>
-      </c>
-      <c r="E2" s="3" t="str">
+      </c>
+      <c r="E2" s="6">
         <f>Forskellige_se!D4</f>
-        <v>4.635</v>
-      </c>
-      <c r="F2" s="3" t="str">
+      </c>
+      <c r="F2" s="6">
         <f>Forskellige_se!G2</f>
-        <v>2.887***</v>
-      </c>
-      <c r="G2" s="3" t="str">
+      </c>
+      <c r="G2" s="6">
         <f>Forskellige_se!H4</f>
-        <v>4.635***</v>
-      </c>
-      <c r="H2" s="3" t="str">
+      </c>
+      <c r="H2" s="6">
         <f>Forskellige_se!I2</f>
-        <v>2.887***</v>
-      </c>
-      <c r="I2" s="3" t="str">
+      </c>
+      <c r="I2" s="6">
         <f>Forskellige_se!J4</f>
-        <v>4.635***</v>
-      </c>
-      <c r="J2" s="3" t="str">
+      </c>
+      <c r="J2" s="6">
         <f>Forskellige_se!K2</f>
-        <v>2.887***</v>
-      </c>
-      <c r="K2" s="3" t="str">
+      </c>
+      <c r="K2" s="6">
         <f>Forskellige_se!L4</f>
-        <v>4.635*</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="4">
         <f>Forskellige_se!A3</f>
-        <v>0.5*h_mse</v>
-      </c>
-      <c r="B3" s="3" t="str">
+      </c>
+      <c r="B3" s="6">
         <f>Forskellige_se!E3</f>
-        <v>(1.057)</v>
-      </c>
-      <c r="C3" s="3" t="str">
+      </c>
+      <c r="C3" s="6">
         <f>Forskellige_se!F5</f>
-        <v>(3.134)</v>
-      </c>
-      <c r="D3" s="3" t="str">
+      </c>
+      <c r="D3" s="6">
         <f>Forskellige_se!C3</f>
-        <v>(1.463)</v>
-      </c>
-      <c r="E3" s="3" t="str">
+      </c>
+      <c r="E3" s="6">
         <f>Forskellige_se!D5</f>
-        <v>(3.976)</v>
-      </c>
-      <c r="F3" s="3" t="str">
+      </c>
+      <c r="F3" s="6">
         <f>Forskellige_se!G3</f>
-        <v>(0.317)</v>
-      </c>
-      <c r="G3" s="3" t="str">
+      </c>
+      <c r="G3" s="6">
         <f>Forskellige_se!H5</f>
-        <v>(0.660)</v>
-      </c>
-      <c r="H3" s="3" t="str">
+      </c>
+      <c r="H3" s="6">
         <f>Forskellige_se!I3</f>
-        <v>(0.465)</v>
-      </c>
-      <c r="I3" s="3" t="str">
+      </c>
+      <c r="I3" s="6">
         <f>Forskellige_se!J5</f>
-        <v>(1.541)</v>
-      </c>
-      <c r="J3" s="3" t="str">
+      </c>
+      <c r="J3" s="6">
         <f>Forskellige_se!K3</f>
-        <v>(1.013)</v>
-      </c>
-      <c r="K3" s="3" t="str">
+      </c>
+      <c r="K3" s="6">
         <f>Forskellige_se!L5</f>
-        <v>(2.484)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="4">
         <f>Forskellige_se!A6</f>
-        <v>h_mse</v>
-      </c>
-      <c r="B4" s="3" t="str">
+      </c>
+      <c r="B4" s="6">
         <f>Forskellige_se!E6</f>
-        <v>0.531</v>
-      </c>
-      <c r="C4" s="3" t="str">
+      </c>
+      <c r="C4" s="6">
         <f>Forskellige_se!F8</f>
-        <v>2.034**</v>
-      </c>
-      <c r="D4" s="3" t="str">
+      </c>
+      <c r="D4" s="6">
         <f>Forskellige_se!C6</f>
-        <v>0.531</v>
-      </c>
-      <c r="E4" s="3" t="str">
+      </c>
+      <c r="E4" s="6">
         <f>Forskellige_se!D8</f>
-        <v>2.034**</v>
-      </c>
-      <c r="F4" s="3" t="str">
+      </c>
+      <c r="F4" s="6">
         <f>Forskellige_se!G6</f>
-        <v>0.531</v>
-      </c>
-      <c r="G4" s="3" t="str">
+      </c>
+      <c r="G4" s="6">
         <f>Forskellige_se!H8</f>
-        <v>2.034***</v>
-      </c>
-      <c r="H4" s="3" t="str">
+      </c>
+      <c r="H4" s="6">
         <f>Forskellige_se!I6</f>
-        <v>0.531**</v>
-      </c>
-      <c r="I4" s="3" t="str">
+      </c>
+      <c r="I4" s="6">
         <f>Forskellige_se!J8</f>
-        <v>2.034***</v>
-      </c>
-      <c r="J4" s="3" t="str">
+      </c>
+      <c r="J4" s="6">
         <f>Forskellige_se!K6</f>
-        <v>0.531</v>
-      </c>
-      <c r="K4" s="3" t="str">
+      </c>
+      <c r="K4" s="6">
         <f>Forskellige_se!L8</f>
-        <v>2.034***</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="4">
         <f>Forskellige_se!A7</f>
-        <v>h_mse</v>
-      </c>
-      <c r="B5" s="3" t="str">
+      </c>
+      <c r="B5" s="6">
         <f>Forskellige_se!E7</f>
-        <v>(0.826)</v>
-      </c>
-      <c r="C5" s="3" t="str">
+      </c>
+      <c r="C5" s="6">
         <f>Forskellige_se!F9</f>
-        <v>(1.012)</v>
-      </c>
-      <c r="D5" s="3" t="str">
+      </c>
+      <c r="D5" s="6">
         <f>Forskellige_se!C7</f>
-        <v>(0.903)</v>
-      </c>
-      <c r="E5" s="3" t="str">
+      </c>
+      <c r="E5" s="6">
         <f>Forskellige_se!D9</f>
-        <v>(0.803)</v>
-      </c>
-      <c r="F5" s="3" t="str">
+      </c>
+      <c r="F5" s="6">
         <f>Forskellige_se!G7</f>
-        <v>(1.121)</v>
-      </c>
-      <c r="G5" s="3" t="str">
+      </c>
+      <c r="G5" s="6">
         <f>Forskellige_se!H9</f>
-        <v>(0.729)</v>
-      </c>
-      <c r="H5" s="3" t="str">
+      </c>
+      <c r="H5" s="6">
         <f>Forskellige_se!I7</f>
-        <v>(0.256)</v>
-      </c>
-      <c r="I5" s="3" t="str">
+      </c>
+      <c r="I5" s="6">
         <f>Forskellige_se!J9</f>
-        <v>(0.381)</v>
-      </c>
-      <c r="J5" s="3" t="str">
+      </c>
+      <c r="J5" s="6">
         <f>Forskellige_se!K7</f>
-        <v>(0.474)</v>
-      </c>
-      <c r="K5" s="3" t="str">
+      </c>
+      <c r="K5" s="6">
         <f>Forskellige_se!L9</f>
-        <v>(0.636)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="4">
         <f>Forskellige_se!A10</f>
-        <v>2*h_mse</v>
-      </c>
-      <c r="B6" s="3" t="str">
+      </c>
+      <c r="B6" s="6">
         <f>Forskellige_se!E10</f>
-        <v>-0.959</v>
-      </c>
-      <c r="C6" s="3" t="str">
+      </c>
+      <c r="C6" s="6">
         <f>Forskellige_se!F12</f>
-        <v>-1.115</v>
-      </c>
-      <c r="D6" s="3" t="str">
+      </c>
+      <c r="D6" s="6">
         <f>Forskellige_se!C10</f>
-        <v>-0.959</v>
-      </c>
-      <c r="E6" s="3" t="str">
+      </c>
+      <c r="E6" s="6">
         <f>Forskellige_se!D12</f>
-        <v>-1.115</v>
-      </c>
-      <c r="F6" s="3" t="str">
+      </c>
+      <c r="F6" s="6">
         <f>Forskellige_se!G10</f>
-        <v>-0.959</v>
-      </c>
-      <c r="G6" s="3" t="str">
+      </c>
+      <c r="G6" s="6">
         <f>Forskellige_se!H12</f>
-        <v>-1.115</v>
-      </c>
-      <c r="H6" s="3" t="str">
+      </c>
+      <c r="H6" s="6">
         <f>Forskellige_se!I10</f>
-        <v>-0.959***</v>
-      </c>
-      <c r="I6" s="3" t="str">
+      </c>
+      <c r="I6" s="6">
         <f>Forskellige_se!J12</f>
-        <v>-1.115***</v>
-      </c>
-      <c r="J6" s="3" t="str">
+      </c>
+      <c r="J6" s="6">
         <f>Forskellige_se!K10</f>
-        <v>-0.959***</v>
-      </c>
-      <c r="K6" s="3" t="str">
+      </c>
+      <c r="K6" s="6">
         <f>Forskellige_se!L12</f>
-        <v>-1.115***</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+      <c r="A7" s="4">
         <f>Forskellige_se!A11</f>
-        <v>2*h_mse</v>
-      </c>
-      <c r="B7" s="3" t="str">
+      </c>
+      <c r="B7" s="6">
         <f>Forskellige_se!E11</f>
-        <v>(0.697)</v>
-      </c>
-      <c r="C7" s="3" t="str">
+      </c>
+      <c r="C7" s="6">
         <f>Forskellige_se!F13</f>
-        <v>(1.235)</v>
-      </c>
-      <c r="D7" s="3" t="str">
+      </c>
+      <c r="D7" s="6">
         <f>Forskellige_se!C11</f>
-        <v>(0.734)</v>
-      </c>
-      <c r="E7" s="3" t="str">
+      </c>
+      <c r="E7" s="6">
         <f>Forskellige_se!D13</f>
-        <v>(1.465)</v>
-      </c>
-      <c r="F7" s="3" t="str">
+      </c>
+      <c r="F7" s="6">
         <f>Forskellige_se!G11</f>
-        <v>(0.756)</v>
-      </c>
-      <c r="G7" s="3" t="str">
+      </c>
+      <c r="G7" s="6">
         <f>Forskellige_se!H13</f>
-        <v>(1.076)</v>
-      </c>
-      <c r="H7" s="3" t="str">
+      </c>
+      <c r="H7" s="6">
         <f>Forskellige_se!I11</f>
-        <v>(0.216)</v>
-      </c>
-      <c r="I7" s="3" t="str">
+      </c>
+      <c r="I7" s="6">
         <f>Forskellige_se!J13</f>
-        <v>(0.352)</v>
-      </c>
-      <c r="J7" s="3" t="str">
+      </c>
+      <c r="J7" s="6">
         <f>Forskellige_se!K11</f>
-        <v>(0.272)</v>
-      </c>
-      <c r="K7" s="3" t="str">
+      </c>
+      <c r="K7" s="6">
         <f>Forskellige_se!L13</f>
-        <v>(0.424)</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -935,337 +853,410 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="7.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="3" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="3" width="11.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="L2" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="L3" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="L6" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="L7" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K10" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="L10" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I11" t="s">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K11" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="L11" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L12" t="s">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L13" t="s">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>